<commit_message>
commited changes for milestones
</commit_message>
<xml_diff>
--- a/milestone 1/rawdata.xlsx
+++ b/milestone 1/rawdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Tracker\milestone 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CC2BFC-6356-4369-B265-331E10D1BB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5135FB-510D-473C-9267-CE2216CDA764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="2964" windowWidth="12924" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="14328" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,16 +126,16 @@
     <t>Duplicate Entry</t>
   </si>
   <si>
-    <t>Study_Hours</t>
-  </si>
-  <si>
-    <t>Sleep_Hours</t>
-  </si>
-  <si>
-    <t>Social_Media_Hours</t>
-  </si>
-  <si>
-    <t>Student_Name</t>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Study Hours</t>
+  </si>
+  <si>
+    <t>Sleep Hours</t>
+  </si>
+  <si>
+    <t>Social Media Hours</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -499,16 +501,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>

</xml_diff>